<commit_message>
Výpis hodnocení ze souboru
</commit_message>
<xml_diff>
--- a/Zadání.xlsx
+++ b/Zadání.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B61F9C5-B7E6-4150-A195-2A8A680AC47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A8CA3-F845-455C-BD19-DDDDA5F39D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,13 +594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="J4">
         <f>COUNTIF(E3:E33,"ne")</f>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(E3:E33,"ano")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="J7">
         <f>SUM(F3:F33)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2023,11 +2023,11 @@
         <v>37</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Základní výpis z databáze + výpis detailů
</commit_message>
<xml_diff>
--- a/Zadání.xlsx
+++ b/Zadání.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A8CA3-F845-455C-BD19-DDDDA5F39D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67973106-3F3A-4DEB-A546-0462676D9E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
   <si>
     <t xml:space="preserve"> Na úvodní stránku umístěte funkci PHP pro zápis aktuálního data</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>ano</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -594,13 +597,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1564,7 +1567,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,7 +1631,7 @@
       </c>
       <c r="J3">
         <f>COUNTIF(E3:E33,"ano")+COUNTIF(E3:E33,"ne")</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1656,7 +1659,7 @@
       </c>
       <c r="J4">
         <f>COUNTIF(E3:E33,"ne")</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1684,7 +1687,7 @@
       </c>
       <c r="J5">
         <f>COUNTIF(E3:E33,"wip")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1712,7 +1715,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(E3:E33,"ano")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,7 +1743,7 @@
       </c>
       <c r="J7">
         <f>SUM(F3:F33)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1868,7 +1871,7 @@
         <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -2065,11 +2068,11 @@
         <v>37</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Změna hesla + samostatný soubor pro session start
</commit_message>
<xml_diff>
--- a/Zadání.xlsx
+++ b/Zadání.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67973106-3F3A-4DEB-A546-0462676D9E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFF3221-8C0C-4CDE-95CF-939C27253278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t xml:space="preserve"> Na úvodní stránku umístěte funkci PHP pro zápis aktuálního data</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t>ano</t>
-  </si>
-  <si>
-    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -266,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -359,11 +356,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -391,6 +419,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -597,10 +628,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -1566,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,7 +1662,7 @@
       </c>
       <c r="J3">
         <f>COUNTIF(E3:E33,"ano")+COUNTIF(E3:E33,"ne")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1659,7 +1690,7 @@
       </c>
       <c r="J4">
         <f>COUNTIF(E3:E33,"ne")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1687,7 +1718,7 @@
       </c>
       <c r="J5">
         <f>COUNTIF(E3:E33,"wip")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1871,7 +1902,7 @@
         <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -2004,7 +2035,7 @@
       <c r="D21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F21">
@@ -2025,7 +2056,7 @@
       <c r="D22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="16" t="s">
         <v>50</v>
       </c>
       <c r="F22">
@@ -2046,7 +2077,7 @@
       <c r="D23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="16" t="s">
         <v>50</v>
       </c>
       <c r="F23">
@@ -2064,10 +2095,10 @@
       <c r="C24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F24">
@@ -2090,13 +2121,13 @@
       <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F26">
@@ -2109,13 +2140,13 @@
       <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F27">
@@ -2130,13 +2161,13 @@
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F28">
@@ -2154,7 +2185,7 @@
       <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="8" t="s">

</xml_diff>

<commit_message>
update výpisu a zadání
</commit_message>
<xml_diff>
--- a/Zadání.xlsx
+++ b/Zadání.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2.RP_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Xampp\htdocs\2.RP_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFF3221-8C0C-4CDE-95CF-939C27253278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F873BEA-F421-425D-A631-1A49BE59DF16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,17 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -413,15 +402,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -527,7 +516,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="cs-CZ"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -628,13 +617,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,7 +680,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="cs-CZ"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -721,7 +710,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="cs-CZ"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1597,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,11 +1603,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
@@ -1690,7 +1679,7 @@
       </c>
       <c r="J4">
         <f>COUNTIF(E3:E33,"ne")</f>
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1746,7 +1735,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(E3:E33,"ano")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1774,7 +1763,7 @@
       </c>
       <c r="J7">
         <f>SUM(F3:F33)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2035,7 +2024,7 @@
       <c r="D21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F21">
@@ -2056,7 +2045,7 @@
       <c r="D22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="14" t="s">
         <v>50</v>
       </c>
       <c r="F22">
@@ -2077,7 +2066,7 @@
       <c r="D23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="14" t="s">
         <v>50</v>
       </c>
       <c r="F23">
@@ -2098,7 +2087,7 @@
       <c r="D24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F24">
@@ -2127,12 +2116,12 @@
       <c r="D26" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>41</v>
+      <c r="E26" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2146,12 +2135,12 @@
       <c r="D27" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>41</v>
+      <c r="E27" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2167,7 +2156,7 @@
       <c r="D28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F28">
@@ -2267,14 +2256,14 @@
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
přidání placeholderů do vyhledávače
</commit_message>
<xml_diff>
--- a/Zadání.xlsx
+++ b/Zadání.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cinedb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cinedb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E25618-42C0-6A43-8378-A30FC7F31ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99657DA-EE0D-4223-8F66-5CCAC8F071BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -252,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -425,6 +420,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -631,13 +627,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,30 +1596,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5" customWidth="1"/>
-    <col min="3" max="3" width="77.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" customWidth="1"/>
-    <col min="7" max="7" width="51.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1640,7 +1636,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1665,10 +1661,10 @@
       </c>
       <c r="J3">
         <f>COUNTIF(E3:E33,"ano")+COUNTIF(E3:E33,"ne")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1693,10 +1689,10 @@
       </c>
       <c r="J4">
         <f>COUNTIF(E3:E33,"ne")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1721,10 +1717,10 @@
       </c>
       <c r="J5">
         <f>COUNTIF(E3:E33,"wip")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1749,10 +1745,10 @@
       </c>
       <c r="J6">
         <f>COUNTIF(E3:E33,"ano")</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1777,10 +1773,10 @@
       </c>
       <c r="J7">
         <f>SUM(F3:F33)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1801,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1822,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1843,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -1862,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4">
         <f>SUM(B3:B11)</f>
@@ -1870,7 +1866,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1891,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1912,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1933,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -1954,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1975,7 +1971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -1996,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -2017,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4">
         <f>SUM(B13:B19)</f>
@@ -2025,7 +2021,7 @@
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -2046,7 +2042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -2088,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -2109,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4">
         <f>SUM(B21:B24)</f>
@@ -2117,7 +2113,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2138,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <v>1</v>
@@ -2157,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2178,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -2191,15 +2187,15 @@
       <c r="D29" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>41</v>
+      <c r="E29" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -2213,14 +2209,14 @@
         <v>39</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -2241,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4">
         <f>SUM(B26:B31)</f>
@@ -2249,7 +2245,7 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4">
         <v>2</v>
@@ -2268,21 +2264,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="16"/>
       <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="16"/>
       <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="6"/>

</xml_diff>